<commit_message>
feat: read excel, not convert to Request objects
</commit_message>
<xml_diff>
--- a/Lenh_Dieu_Xe.xlsx
+++ b/Lenh_Dieu_Xe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tung\Projects\Project-70m\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80549B36-A1B1-481F-89F4-F93BC55F3386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF34157D-D59F-4060-B935-B1BD8156D46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19022025" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="258">
   <si>
     <t>Mã số: BM 01-QT 01-ĐX
 Ngày hiệu lực:25 – 08 -2022
@@ -44,7 +44,7 @@
     <t>STT</t>
   </si>
   <si>
-    <t>Khách hàng</t>
+    <t>KHÁCH HÀNG</t>
   </si>
   <si>
     <t>THỂ TÍCH (M3)</t>
@@ -104,13 +104,13 @@
     <t>☑</t>
   </si>
   <si>
-    <t>Thảo Nguyễn</t>
-  </si>
-  <si>
-    <t>214956201795</t>
-  </si>
-  <si>
-    <t>+84 41 0263542</t>
+    <t>Bảo Đức Mai</t>
+  </si>
+  <si>
+    <t>020193455554</t>
+  </si>
+  <si>
+    <t>07 8402 9889</t>
   </si>
   <si>
     <t>5t = 26.7m3</t>
@@ -119,13 +119,13 @@
     <t>T(19:00-&gt;23:00)</t>
   </si>
   <si>
-    <t>Nhật Mai Dương</t>
-  </si>
-  <si>
-    <t>417621500636</t>
-  </si>
-  <si>
-    <t>(01) 8204 4469</t>
+    <t>Quý ông Minh Phạm</t>
+  </si>
+  <si>
+    <t>123008870433</t>
+  </si>
+  <si>
+    <t>+84-76-869 0367</t>
   </si>
   <si>
     <t>7t = 32m3</t>
@@ -134,13 +134,13 @@
     <t>D(00:30-&gt;04:30)</t>
   </si>
   <si>
-    <t>Cô Nhật Nguyễn</t>
-  </si>
-  <si>
-    <t>961832300294</t>
-  </si>
-  <si>
-    <t>(09) 0371 5425</t>
+    <t>Mai Bùi</t>
+  </si>
+  <si>
+    <t>647320872419</t>
+  </si>
+  <si>
+    <t>00 1340 3552</t>
   </si>
   <si>
     <t>9t = 38.2m3</t>
@@ -149,25 +149,25 @@
     <t>Báo sau</t>
   </si>
   <si>
-    <t>Hoàng Trần</t>
-  </si>
-  <si>
-    <t>521512882609</t>
-  </si>
-  <si>
-    <t>+84-66-543333</t>
+    <t>An Bảo Dương</t>
+  </si>
+  <si>
+    <t>486685879909</t>
+  </si>
+  <si>
+    <t>+84-64-255 0409</t>
   </si>
   <si>
     <t>12t = 54m3</t>
   </si>
   <si>
-    <t>Chị Khoa Mai</t>
-  </si>
-  <si>
-    <t>943006405720</t>
-  </si>
-  <si>
-    <t>(07)411-0877</t>
+    <t>Thảo Dương</t>
+  </si>
+  <si>
+    <t>067182973349</t>
+  </si>
+  <si>
+    <t>(02) 5176 7462</t>
   </si>
   <si>
     <t>X1</t>
@@ -719,31 +719,31 @@
     <t>Nguyễn Văn A</t>
   </si>
   <si>
-    <t>0611519692</t>
+    <t>0257671614</t>
   </si>
   <si>
     <t>Trần Thị B</t>
   </si>
   <si>
-    <t>0657113779</t>
+    <t>0572707764</t>
   </si>
   <si>
     <t>Lê Văn C</t>
   </si>
   <si>
-    <t>0906427539</t>
+    <t>0425884014</t>
   </si>
   <si>
     <t>Phạm Thị D</t>
   </si>
   <si>
-    <t>0773561436</t>
+    <t>0722297545</t>
   </si>
   <si>
     <t>Hoàng Văn E</t>
   </si>
   <si>
-    <t>0766922762</t>
+    <t>0342388298</t>
   </si>
   <si>
     <t>Thông tin tài xế</t>
@@ -770,34 +770,40 @@
     <t>available</t>
   </si>
   <si>
-    <t>967979358234</t>
-  </si>
-  <si>
-    <t>29A-61011</t>
-  </si>
-  <si>
-    <t>693971104527</t>
-  </si>
-  <si>
-    <t>29A-60263</t>
-  </si>
-  <si>
-    <t>182906085845</t>
-  </si>
-  <si>
-    <t>29A-98438</t>
-  </si>
-  <si>
-    <t>988961206129</t>
-  </si>
-  <si>
-    <t>29A-78746</t>
-  </si>
-  <si>
-    <t>133825532740</t>
-  </si>
-  <si>
-    <t>29A-16302</t>
+    <t>202708715415</t>
+  </si>
+  <si>
+    <t>29A-45860</t>
+  </si>
+  <si>
+    <t>708924147975</t>
+  </si>
+  <si>
+    <t>29A-63224</t>
+  </si>
+  <si>
+    <t>302732700760</t>
+  </si>
+  <si>
+    <t>29A-32125</t>
+  </si>
+  <si>
+    <t>475420041480</t>
+  </si>
+  <si>
+    <t>29A-89692</t>
+  </si>
+  <si>
+    <t>355657867599</t>
+  </si>
+  <si>
+    <t>29A-83249</t>
+  </si>
+  <si>
+    <t>kugsfjlhgusyEFGLUISGDF</t>
+  </si>
+  <si>
+    <t>LHIDHFSLJBGFDIUHUH</t>
   </si>
 </sst>
 </file>
@@ -808,7 +814,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,60 +848,19 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="14"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="163"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -907,32 +872,11 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -955,7 +899,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1042,48 +986,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1101,102 +1008,56 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1524,17 +1385,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q11825"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="43.6640625" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="14.88671875" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" customWidth="1"/>
@@ -1547,33 +1409,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="44" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="45"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1621,20 +1483,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
       <c r="B5" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
+      <c r="C5" s="7">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -1642,20 +1524,40 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+    <row r="6" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
       <c r="B6" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="C6" s="7">
+        <v>20</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -1663,20 +1565,18 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="14"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -1684,58 +1584,56 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="21"/>
+    <row r="8" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16"/>
+    <row r="9" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="22"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="14"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -1743,18 +1641,18 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1762,73 +1660,73 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16"/>
+    <row r="12" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="22"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="14"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="26"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
+    <row r="14" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16"/>
+    <row r="15" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -1836,18 +1734,18 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16"/>
+    <row r="16" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -1855,18 +1753,18 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
+    <row r="17" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="14"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -1874,18 +1772,18 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="16"/>
+    <row r="18" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="14"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1893,18 +1791,18 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="14"/>
+    <row r="19" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -1912,18 +1810,18 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="14"/>
+    <row r="20" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -1931,18 +1829,18 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="14"/>
+    <row r="21" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="12"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -1950,18 +1848,18 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="14"/>
+    <row r="22" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1969,18 +1867,18 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
-    <row r="23" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="16"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="14"/>
+    <row r="23" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="11"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -1988,18 +1886,18 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="16"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="14"/>
+    <row r="24" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="11"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -2007,18 +1905,18 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="16"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="14"/>
+    <row r="25" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -2026,18 +1924,18 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
-    <row r="26" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="14"/>
+    <row r="26" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="12"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -2045,18 +1943,18 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
     </row>
-    <row r="27" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="14"/>
+    <row r="27" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="12"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="11"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
@@ -2064,18 +1962,18 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
     </row>
-    <row r="28" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="14"/>
+    <row r="28" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="11"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
@@ -2083,18 +1981,18 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
     </row>
-    <row r="29" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="16"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="14"/>
+    <row r="29" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="12"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="11"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
@@ -2102,18 +2000,18 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
     </row>
-    <row r="30" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="16"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="14"/>
+    <row r="30" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
@@ -2121,18 +2019,18 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
     </row>
-    <row r="31" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="16"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="14"/>
+    <row r="31" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="12"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="11"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
@@ -2140,18 +2038,18 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
     </row>
-    <row r="32" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="16"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="14"/>
+    <row r="32" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="11"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
@@ -2159,18 +2057,18 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
     </row>
-    <row r="33" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="14"/>
+    <row r="33" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="12"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="11"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -2178,18 +2076,18 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
     </row>
-    <row r="34" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="14"/>
+    <row r="34" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="12"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="11"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -2197,18 +2095,18 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
     </row>
-    <row r="35" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="16"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="14"/>
+    <row r="35" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="12"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="11"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -2216,18 +2114,18 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
     </row>
-    <row r="36" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="14"/>
+    <row r="36" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="12"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="11"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -2235,18 +2133,18 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
     </row>
-    <row r="37" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="16"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="14"/>
+    <row r="37" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="12"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="11"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
@@ -2254,18 +2152,18 @@
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
     </row>
-    <row r="38" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="16"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="14"/>
+    <row r="38" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="12"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="11"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -2273,18 +2171,18 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
     </row>
-    <row r="39" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="16"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="14"/>
+    <row r="39" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="12"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="11"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -2292,272 +2190,272 @@
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
     </row>
-    <row r="40" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="16"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="14"/>
+    <row r="40" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="12"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="11"/>
       <c r="L40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
     </row>
-    <row r="41" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="22"/>
+    <row r="41" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="12"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="14"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
     </row>
-    <row r="42" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="18"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
     </row>
-    <row r="43" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="16"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="36"/>
+    <row r="43" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="12"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="21"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
     </row>
-    <row r="44" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="35"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="12"/>
       <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
+      <c r="L44" s="18"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
     </row>
-    <row r="45" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="16"/>
+    <row r="45" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="12"/>
       <c r="B45" s="8"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="7"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="18"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
     </row>
-    <row r="46" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="16"/>
+    <row r="46" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="12"/>
       <c r="B46" s="8"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="7"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="18"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
     </row>
-    <row r="47" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="7"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="18"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
     </row>
-    <row r="48" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="7"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="10"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="8"/>
       <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
+      <c r="L48" s="18"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
     </row>
-    <row r="49" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="10"/>
+    <row r="49" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="8"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="24"/>
-      <c r="K49" s="14"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="11"/>
       <c r="L49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
     </row>
-    <row r="50" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="16"/>
+    <row r="50" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="12"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="11"/>
       <c r="L50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
     </row>
-    <row r="51" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="7"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="18"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
     </row>
-    <row r="52" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="16"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="7"/>
+    <row r="52" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="12"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="18"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
     </row>
-    <row r="53" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="16"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="22"/>
+    <row r="53" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="12"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="14"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
     </row>
-    <row r="54" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="16"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="14"/>
+    <row r="54" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="12"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="11"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
@@ -2565,19 +2463,19 @@
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
     </row>
-    <row r="55" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="40"/>
+    <row r="55" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="24"/>
     </row>
     <row r="11825" spans="17:17" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Q11825" s="3">
@@ -2591,17 +2489,20 @@
     <mergeCell ref="B1:H2"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" sqref="E5:E55" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"S(08:00-&gt;12:00),C(13:30-&gt;17:30),T(19:00-&gt;23:00),D(00:30-&gt;04:30),Báo sau"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I5:I55 J5:J55 K5:K55" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"☐,☑"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H5:H55" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"Thảo Nguyễn,Nhật Mai Dương,Cô Nhật Nguyễn,Hoàng Trần,Chị Khoa Mai"</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="G5:G55" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>"X1,X4,VAC,X5,X6,X7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D5:D55" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" sqref="H5:H55" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>"Bảo Đức Mai,Quý ông Minh Phạm,Mai Bùi,An Bảo Dương,Thảo Dương"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D5:D55" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"1.4t = 9.7m3,3.5t = 24.2m3,5t = 26.7m3,7t = 32m3,9t = 38.2m3,12t = 54m3"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2635,16 +2536,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="F1" s="41" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="F1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="41" t="s">
+      <c r="AA1" s="25" t="s">
         <v>16</v>
       </c>
       <c r="AB1" t="s">
@@ -2664,10 +2565,10 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="41" t="s">
+      <c r="AA2" s="25" t="s">
         <v>22</v>
       </c>
       <c r="AB2" t="s">
@@ -2687,10 +2588,10 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="41" t="s">
+      <c r="AA3" s="25" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2707,10 +2608,10 @@
       <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AA4" s="41" t="s">
+      <c r="AA4" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2727,10 +2628,10 @@
       <c r="D5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="AA5" s="41" t="s">
+      <c r="AA5" s="25" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2747,7 +2648,7 @@
       <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="25" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2777,7 +2678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3450,59 +3351,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
-      <c r="AW1" s="53"/>
-      <c r="AX1" s="53"/>
-      <c r="AY1" s="53"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3514,62 +3415,62 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53" t="s">
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53" t="s">
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
-      <c r="AW2" s="53"/>
-      <c r="AX2" s="53"/>
-      <c r="AY2" s="53"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -3581,14 +3482,14 @@
       <c r="C3" t="s">
         <v>229</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="42"/>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="42"/>
-      <c r="AM3" s="43"/>
-      <c r="AN3" s="42"/>
-      <c r="AY3" s="43"/>
+      <c r="D3" s="26"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="26"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="26"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="26"/>
+      <c r="AY3" s="27"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3600,14 +3501,14 @@
       <c r="C4" t="s">
         <v>231</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="42"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="42"/>
-      <c r="AM4" s="43"/>
-      <c r="AN4" s="42"/>
-      <c r="AY4" s="43"/>
+      <c r="D4" s="26"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="26"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="26"/>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="26"/>
+      <c r="AY4" s="27"/>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -3619,14 +3520,14 @@
       <c r="C5" t="s">
         <v>233</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="42"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="42"/>
-      <c r="AM5" s="43"/>
-      <c r="AN5" s="42"/>
-      <c r="AY5" s="43"/>
+      <c r="D5" s="26"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="26"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="26"/>
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="26"/>
+      <c r="AY5" s="27"/>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -3638,14 +3539,14 @@
       <c r="C6" t="s">
         <v>235</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="42"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="42"/>
-      <c r="AM6" s="43"/>
-      <c r="AN6" s="42"/>
-      <c r="AY6" s="43"/>
+      <c r="D6" s="26"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="26"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="26"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="26"/>
+      <c r="AY6" s="27"/>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -3657,944 +3558,944 @@
       <c r="C7" t="s">
         <v>237</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="42"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="42"/>
-      <c r="AM7" s="43"/>
-      <c r="AN7" s="42"/>
-      <c r="AY7" s="43"/>
+      <c r="D7" s="26"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="26"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="26"/>
+      <c r="AM7" s="27"/>
+      <c r="AN7" s="26"/>
+      <c r="AY7" s="27"/>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D8" s="42"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="42"/>
-      <c r="AA8" s="43"/>
-      <c r="AB8" s="42"/>
-      <c r="AM8" s="43"/>
-      <c r="AN8" s="42"/>
-      <c r="AY8" s="43"/>
+      <c r="D8" s="26"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="26"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="26"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="26"/>
+      <c r="AY8" s="27"/>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D9" s="42"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="42"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="42"/>
-      <c r="AM9" s="43"/>
-      <c r="AN9" s="42"/>
-      <c r="AY9" s="43"/>
+      <c r="D9" s="26"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="26"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="26"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="26"/>
+      <c r="AY9" s="27"/>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D10" s="42"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="42"/>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="42"/>
-      <c r="AM10" s="43"/>
-      <c r="AN10" s="42"/>
-      <c r="AY10" s="43"/>
+      <c r="D10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="26"/>
+      <c r="AA10" s="27"/>
+      <c r="AB10" s="26"/>
+      <c r="AM10" s="27"/>
+      <c r="AN10" s="26"/>
+      <c r="AY10" s="27"/>
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D11" s="42"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="42"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="42"/>
-      <c r="AM11" s="43"/>
-      <c r="AN11" s="42"/>
-      <c r="AY11" s="43"/>
+      <c r="D11" s="26"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="26"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="26"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="26"/>
+      <c r="AY11" s="27"/>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D12" s="42"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="42"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="42"/>
-      <c r="AM12" s="43"/>
-      <c r="AN12" s="42"/>
-      <c r="AY12" s="43"/>
+      <c r="D12" s="26"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="26"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="26"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="26"/>
+      <c r="AY12" s="27"/>
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D13" s="42"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="42"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="42"/>
-      <c r="AM13" s="43"/>
-      <c r="AN13" s="42"/>
-      <c r="AY13" s="43"/>
+      <c r="D13" s="26"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="26"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="26"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="26"/>
+      <c r="AY13" s="27"/>
     </row>
     <row r="14" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D14" s="42"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="42"/>
-      <c r="AA14" s="43"/>
-      <c r="AB14" s="42"/>
-      <c r="AM14" s="43"/>
-      <c r="AN14" s="42"/>
-      <c r="AY14" s="43"/>
+      <c r="D14" s="26"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="26"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="26"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="26"/>
+      <c r="AY14" s="27"/>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D15" s="42"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="42"/>
-      <c r="AA15" s="43"/>
-      <c r="AB15" s="42"/>
-      <c r="AM15" s="43"/>
-      <c r="AN15" s="42"/>
-      <c r="AY15" s="43"/>
+      <c r="D15" s="26"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="26"/>
+      <c r="AA15" s="27"/>
+      <c r="AB15" s="26"/>
+      <c r="AM15" s="27"/>
+      <c r="AN15" s="26"/>
+      <c r="AY15" s="27"/>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="D16" s="42"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="42"/>
-      <c r="AA16" s="43"/>
-      <c r="AB16" s="42"/>
-      <c r="AM16" s="43"/>
-      <c r="AN16" s="42"/>
-      <c r="AY16" s="43"/>
+      <c r="D16" s="26"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="26"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="26"/>
+      <c r="AM16" s="27"/>
+      <c r="AN16" s="26"/>
+      <c r="AY16" s="27"/>
     </row>
     <row r="17" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D17" s="42"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="42"/>
-      <c r="AA17" s="43"/>
-      <c r="AB17" s="42"/>
-      <c r="AM17" s="43"/>
-      <c r="AN17" s="42"/>
-      <c r="AY17" s="43"/>
+      <c r="D17" s="26"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="26"/>
+      <c r="AA17" s="27"/>
+      <c r="AB17" s="26"/>
+      <c r="AM17" s="27"/>
+      <c r="AN17" s="26"/>
+      <c r="AY17" s="27"/>
     </row>
     <row r="18" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D18" s="42"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="42"/>
-      <c r="AA18" s="43"/>
-      <c r="AB18" s="42"/>
-      <c r="AM18" s="43"/>
-      <c r="AN18" s="42"/>
-      <c r="AY18" s="43"/>
+      <c r="D18" s="26"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="26"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="26"/>
+      <c r="AM18" s="27"/>
+      <c r="AN18" s="26"/>
+      <c r="AY18" s="27"/>
     </row>
     <row r="19" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D19" s="42"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="42"/>
-      <c r="AA19" s="43"/>
-      <c r="AB19" s="42"/>
-      <c r="AM19" s="43"/>
-      <c r="AN19" s="42"/>
-      <c r="AY19" s="43"/>
+      <c r="D19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="26"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="26"/>
+      <c r="AM19" s="27"/>
+      <c r="AN19" s="26"/>
+      <c r="AY19" s="27"/>
     </row>
     <row r="20" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D20" s="42"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="42"/>
-      <c r="AA20" s="43"/>
-      <c r="AB20" s="42"/>
-      <c r="AM20" s="43"/>
-      <c r="AN20" s="42"/>
-      <c r="AY20" s="43"/>
+      <c r="D20" s="26"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="26"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="26"/>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="26"/>
+      <c r="AY20" s="27"/>
     </row>
     <row r="21" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D21" s="42"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="42"/>
-      <c r="AA21" s="43"/>
-      <c r="AB21" s="42"/>
-      <c r="AM21" s="43"/>
-      <c r="AN21" s="42"/>
-      <c r="AY21" s="43"/>
+      <c r="D21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="26"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="26"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="26"/>
+      <c r="AY21" s="27"/>
     </row>
     <row r="22" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D22" s="42"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="42"/>
-      <c r="AA22" s="43"/>
-      <c r="AB22" s="42"/>
-      <c r="AM22" s="43"/>
-      <c r="AN22" s="42"/>
-      <c r="AY22" s="43"/>
+      <c r="D22" s="26"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="26"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="26"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="26"/>
+      <c r="AY22" s="27"/>
     </row>
     <row r="23" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D23" s="42"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="42"/>
-      <c r="AA23" s="43"/>
-      <c r="AB23" s="42"/>
-      <c r="AM23" s="43"/>
-      <c r="AN23" s="42"/>
-      <c r="AY23" s="43"/>
+      <c r="D23" s="26"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="26"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="26"/>
+      <c r="AM23" s="27"/>
+      <c r="AN23" s="26"/>
+      <c r="AY23" s="27"/>
     </row>
     <row r="24" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D24" s="42"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="42"/>
-      <c r="AA24" s="43"/>
-      <c r="AB24" s="42"/>
-      <c r="AM24" s="43"/>
-      <c r="AN24" s="42"/>
-      <c r="AY24" s="43"/>
+      <c r="D24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="26"/>
+      <c r="AA24" s="27"/>
+      <c r="AB24" s="26"/>
+      <c r="AM24" s="27"/>
+      <c r="AN24" s="26"/>
+      <c r="AY24" s="27"/>
     </row>
     <row r="25" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D25" s="42"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="42"/>
-      <c r="AA25" s="43"/>
-      <c r="AB25" s="42"/>
-      <c r="AM25" s="43"/>
-      <c r="AN25" s="42"/>
-      <c r="AY25" s="43"/>
+      <c r="D25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="26"/>
+      <c r="AA25" s="27"/>
+      <c r="AB25" s="26"/>
+      <c r="AM25" s="27"/>
+      <c r="AN25" s="26"/>
+      <c r="AY25" s="27"/>
     </row>
     <row r="26" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D26" s="42"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="42"/>
-      <c r="AA26" s="43"/>
-      <c r="AB26" s="42"/>
-      <c r="AM26" s="43"/>
-      <c r="AN26" s="42"/>
-      <c r="AY26" s="43"/>
+      <c r="D26" s="26"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="26"/>
+      <c r="AA26" s="27"/>
+      <c r="AB26" s="26"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="26"/>
+      <c r="AY26" s="27"/>
     </row>
     <row r="27" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D27" s="42"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="42"/>
-      <c r="AA27" s="43"/>
-      <c r="AB27" s="42"/>
-      <c r="AM27" s="43"/>
-      <c r="AN27" s="42"/>
-      <c r="AY27" s="43"/>
+      <c r="D27" s="26"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="26"/>
+      <c r="AA27" s="27"/>
+      <c r="AB27" s="26"/>
+      <c r="AM27" s="27"/>
+      <c r="AN27" s="26"/>
+      <c r="AY27" s="27"/>
     </row>
     <row r="28" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D28" s="42"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="42"/>
-      <c r="AA28" s="43"/>
-      <c r="AB28" s="42"/>
-      <c r="AM28" s="43"/>
-      <c r="AN28" s="42"/>
-      <c r="AY28" s="43"/>
+      <c r="D28" s="26"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="26"/>
+      <c r="AA28" s="27"/>
+      <c r="AB28" s="26"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="26"/>
+      <c r="AY28" s="27"/>
     </row>
     <row r="29" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D29" s="42"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="42"/>
-      <c r="AA29" s="43"/>
-      <c r="AB29" s="42"/>
-      <c r="AM29" s="43"/>
-      <c r="AN29" s="42"/>
-      <c r="AY29" s="43"/>
+      <c r="D29" s="26"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="26"/>
+      <c r="AA29" s="27"/>
+      <c r="AB29" s="26"/>
+      <c r="AM29" s="27"/>
+      <c r="AN29" s="26"/>
+      <c r="AY29" s="27"/>
     </row>
     <row r="30" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D30" s="42"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="42"/>
-      <c r="AA30" s="43"/>
-      <c r="AB30" s="42"/>
-      <c r="AM30" s="43"/>
-      <c r="AN30" s="42"/>
-      <c r="AY30" s="43"/>
+      <c r="D30" s="26"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="26"/>
+      <c r="AA30" s="27"/>
+      <c r="AB30" s="26"/>
+      <c r="AM30" s="27"/>
+      <c r="AN30" s="26"/>
+      <c r="AY30" s="27"/>
     </row>
     <row r="31" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D31" s="42"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="42"/>
-      <c r="AA31" s="43"/>
-      <c r="AB31" s="42"/>
-      <c r="AM31" s="43"/>
-      <c r="AN31" s="42"/>
-      <c r="AY31" s="43"/>
+      <c r="D31" s="26"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="26"/>
+      <c r="AA31" s="27"/>
+      <c r="AB31" s="26"/>
+      <c r="AM31" s="27"/>
+      <c r="AN31" s="26"/>
+      <c r="AY31" s="27"/>
     </row>
     <row r="32" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D32" s="42"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="42"/>
-      <c r="AA32" s="43"/>
-      <c r="AB32" s="42"/>
-      <c r="AM32" s="43"/>
-      <c r="AN32" s="42"/>
-      <c r="AY32" s="43"/>
+      <c r="D32" s="26"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="26"/>
+      <c r="AA32" s="27"/>
+      <c r="AB32" s="26"/>
+      <c r="AM32" s="27"/>
+      <c r="AN32" s="26"/>
+      <c r="AY32" s="27"/>
     </row>
     <row r="33" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D33" s="42"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="42"/>
-      <c r="AA33" s="43"/>
-      <c r="AB33" s="42"/>
-      <c r="AM33" s="43"/>
-      <c r="AN33" s="42"/>
-      <c r="AY33" s="43"/>
+      <c r="D33" s="26"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="26"/>
+      <c r="AA33" s="27"/>
+      <c r="AB33" s="26"/>
+      <c r="AM33" s="27"/>
+      <c r="AN33" s="26"/>
+      <c r="AY33" s="27"/>
     </row>
     <row r="34" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D34" s="42"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="42"/>
-      <c r="AA34" s="43"/>
-      <c r="AB34" s="42"/>
-      <c r="AM34" s="43"/>
-      <c r="AN34" s="42"/>
-      <c r="AY34" s="43"/>
+      <c r="D34" s="26"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="26"/>
+      <c r="AA34" s="27"/>
+      <c r="AB34" s="26"/>
+      <c r="AM34" s="27"/>
+      <c r="AN34" s="26"/>
+      <c r="AY34" s="27"/>
     </row>
     <row r="35" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D35" s="42"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="42"/>
-      <c r="AA35" s="43"/>
-      <c r="AB35" s="42"/>
-      <c r="AM35" s="43"/>
-      <c r="AN35" s="42"/>
-      <c r="AY35" s="43"/>
+      <c r="D35" s="26"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="26"/>
+      <c r="AA35" s="27"/>
+      <c r="AB35" s="26"/>
+      <c r="AM35" s="27"/>
+      <c r="AN35" s="26"/>
+      <c r="AY35" s="27"/>
     </row>
     <row r="36" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D36" s="42"/>
-      <c r="O36" s="43"/>
-      <c r="P36" s="42"/>
-      <c r="AA36" s="43"/>
-      <c r="AB36" s="42"/>
-      <c r="AM36" s="43"/>
-      <c r="AN36" s="42"/>
-      <c r="AY36" s="43"/>
+      <c r="D36" s="26"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="26"/>
+      <c r="AA36" s="27"/>
+      <c r="AB36" s="26"/>
+      <c r="AM36" s="27"/>
+      <c r="AN36" s="26"/>
+      <c r="AY36" s="27"/>
     </row>
     <row r="37" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D37" s="42"/>
-      <c r="O37" s="43"/>
-      <c r="P37" s="42"/>
-      <c r="AA37" s="43"/>
-      <c r="AB37" s="42"/>
-      <c r="AM37" s="43"/>
-      <c r="AN37" s="42"/>
-      <c r="AY37" s="43"/>
+      <c r="D37" s="26"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="26"/>
+      <c r="AA37" s="27"/>
+      <c r="AB37" s="26"/>
+      <c r="AM37" s="27"/>
+      <c r="AN37" s="26"/>
+      <c r="AY37" s="27"/>
     </row>
     <row r="38" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D38" s="42"/>
-      <c r="O38" s="43"/>
-      <c r="P38" s="42"/>
-      <c r="AA38" s="43"/>
-      <c r="AB38" s="42"/>
-      <c r="AM38" s="43"/>
-      <c r="AN38" s="42"/>
-      <c r="AY38" s="43"/>
+      <c r="D38" s="26"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="26"/>
+      <c r="AA38" s="27"/>
+      <c r="AB38" s="26"/>
+      <c r="AM38" s="27"/>
+      <c r="AN38" s="26"/>
+      <c r="AY38" s="27"/>
     </row>
     <row r="39" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D39" s="42"/>
-      <c r="O39" s="43"/>
-      <c r="P39" s="42"/>
-      <c r="AA39" s="43"/>
-      <c r="AB39" s="42"/>
-      <c r="AM39" s="43"/>
-      <c r="AN39" s="42"/>
-      <c r="AY39" s="43"/>
+      <c r="D39" s="26"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="26"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="26"/>
+      <c r="AM39" s="27"/>
+      <c r="AN39" s="26"/>
+      <c r="AY39" s="27"/>
     </row>
     <row r="40" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D40" s="42"/>
-      <c r="O40" s="43"/>
-      <c r="P40" s="42"/>
-      <c r="AA40" s="43"/>
-      <c r="AB40" s="42"/>
-      <c r="AM40" s="43"/>
-      <c r="AN40" s="42"/>
-      <c r="AY40" s="43"/>
+      <c r="D40" s="26"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="26"/>
+      <c r="AA40" s="27"/>
+      <c r="AB40" s="26"/>
+      <c r="AM40" s="27"/>
+      <c r="AN40" s="26"/>
+      <c r="AY40" s="27"/>
     </row>
     <row r="41" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D41" s="42"/>
-      <c r="O41" s="43"/>
-      <c r="P41" s="42"/>
-      <c r="AA41" s="43"/>
-      <c r="AB41" s="42"/>
-      <c r="AM41" s="43"/>
-      <c r="AN41" s="42"/>
-      <c r="AY41" s="43"/>
+      <c r="D41" s="26"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="26"/>
+      <c r="AA41" s="27"/>
+      <c r="AB41" s="26"/>
+      <c r="AM41" s="27"/>
+      <c r="AN41" s="26"/>
+      <c r="AY41" s="27"/>
     </row>
     <row r="42" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D42" s="42"/>
-      <c r="O42" s="43"/>
-      <c r="P42" s="42"/>
-      <c r="AA42" s="43"/>
-      <c r="AB42" s="42"/>
-      <c r="AM42" s="43"/>
-      <c r="AN42" s="42"/>
-      <c r="AY42" s="43"/>
+      <c r="D42" s="26"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="26"/>
+      <c r="AA42" s="27"/>
+      <c r="AB42" s="26"/>
+      <c r="AM42" s="27"/>
+      <c r="AN42" s="26"/>
+      <c r="AY42" s="27"/>
     </row>
     <row r="43" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D43" s="42"/>
-      <c r="O43" s="43"/>
-      <c r="P43" s="42"/>
-      <c r="AA43" s="43"/>
-      <c r="AB43" s="42"/>
-      <c r="AM43" s="43"/>
-      <c r="AN43" s="42"/>
-      <c r="AY43" s="43"/>
+      <c r="D43" s="26"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="26"/>
+      <c r="AA43" s="27"/>
+      <c r="AB43" s="26"/>
+      <c r="AM43" s="27"/>
+      <c r="AN43" s="26"/>
+      <c r="AY43" s="27"/>
     </row>
     <row r="44" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D44" s="42"/>
-      <c r="O44" s="43"/>
-      <c r="P44" s="42"/>
-      <c r="AA44" s="43"/>
-      <c r="AB44" s="42"/>
-      <c r="AM44" s="43"/>
-      <c r="AN44" s="42"/>
-      <c r="AY44" s="43"/>
+      <c r="D44" s="26"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="26"/>
+      <c r="AA44" s="27"/>
+      <c r="AB44" s="26"/>
+      <c r="AM44" s="27"/>
+      <c r="AN44" s="26"/>
+      <c r="AY44" s="27"/>
     </row>
     <row r="45" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D45" s="42"/>
-      <c r="O45" s="43"/>
-      <c r="P45" s="42"/>
-      <c r="AA45" s="43"/>
-      <c r="AB45" s="42"/>
-      <c r="AM45" s="43"/>
-      <c r="AN45" s="42"/>
-      <c r="AY45" s="43"/>
+      <c r="D45" s="26"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="26"/>
+      <c r="AA45" s="27"/>
+      <c r="AB45" s="26"/>
+      <c r="AM45" s="27"/>
+      <c r="AN45" s="26"/>
+      <c r="AY45" s="27"/>
     </row>
     <row r="46" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D46" s="42"/>
-      <c r="O46" s="43"/>
-      <c r="P46" s="42"/>
-      <c r="AA46" s="43"/>
-      <c r="AB46" s="42"/>
-      <c r="AM46" s="43"/>
-      <c r="AN46" s="42"/>
-      <c r="AY46" s="43"/>
+      <c r="D46" s="26"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="26"/>
+      <c r="AA46" s="27"/>
+      <c r="AB46" s="26"/>
+      <c r="AM46" s="27"/>
+      <c r="AN46" s="26"/>
+      <c r="AY46" s="27"/>
     </row>
     <row r="47" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D47" s="42"/>
-      <c r="O47" s="43"/>
-      <c r="P47" s="42"/>
-      <c r="AA47" s="43"/>
-      <c r="AB47" s="42"/>
-      <c r="AM47" s="43"/>
-      <c r="AN47" s="42"/>
-      <c r="AY47" s="43"/>
+      <c r="D47" s="26"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="26"/>
+      <c r="AA47" s="27"/>
+      <c r="AB47" s="26"/>
+      <c r="AM47" s="27"/>
+      <c r="AN47" s="26"/>
+      <c r="AY47" s="27"/>
     </row>
     <row r="48" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D48" s="42"/>
-      <c r="O48" s="43"/>
-      <c r="P48" s="42"/>
-      <c r="AA48" s="43"/>
-      <c r="AB48" s="42"/>
-      <c r="AM48" s="43"/>
-      <c r="AN48" s="42"/>
-      <c r="AY48" s="43"/>
+      <c r="D48" s="26"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="26"/>
+      <c r="AA48" s="27"/>
+      <c r="AB48" s="26"/>
+      <c r="AM48" s="27"/>
+      <c r="AN48" s="26"/>
+      <c r="AY48" s="27"/>
     </row>
     <row r="49" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D49" s="42"/>
-      <c r="O49" s="43"/>
-      <c r="P49" s="42"/>
-      <c r="AA49" s="43"/>
-      <c r="AB49" s="42"/>
-      <c r="AM49" s="43"/>
-      <c r="AN49" s="42"/>
-      <c r="AY49" s="43"/>
+      <c r="D49" s="26"/>
+      <c r="O49" s="27"/>
+      <c r="P49" s="26"/>
+      <c r="AA49" s="27"/>
+      <c r="AB49" s="26"/>
+      <c r="AM49" s="27"/>
+      <c r="AN49" s="26"/>
+      <c r="AY49" s="27"/>
     </row>
     <row r="50" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D50" s="42"/>
-      <c r="O50" s="43"/>
-      <c r="P50" s="42"/>
-      <c r="AA50" s="43"/>
-      <c r="AB50" s="42"/>
-      <c r="AM50" s="43"/>
-      <c r="AN50" s="42"/>
-      <c r="AY50" s="43"/>
+      <c r="D50" s="26"/>
+      <c r="O50" s="27"/>
+      <c r="P50" s="26"/>
+      <c r="AA50" s="27"/>
+      <c r="AB50" s="26"/>
+      <c r="AM50" s="27"/>
+      <c r="AN50" s="26"/>
+      <c r="AY50" s="27"/>
     </row>
     <row r="51" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D51" s="42"/>
-      <c r="O51" s="43"/>
-      <c r="P51" s="42"/>
-      <c r="AA51" s="43"/>
-      <c r="AB51" s="42"/>
-      <c r="AM51" s="43"/>
-      <c r="AN51" s="42"/>
-      <c r="AY51" s="43"/>
+      <c r="D51" s="26"/>
+      <c r="O51" s="27"/>
+      <c r="P51" s="26"/>
+      <c r="AA51" s="27"/>
+      <c r="AB51" s="26"/>
+      <c r="AM51" s="27"/>
+      <c r="AN51" s="26"/>
+      <c r="AY51" s="27"/>
     </row>
     <row r="52" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D52" s="42"/>
-      <c r="O52" s="43"/>
-      <c r="P52" s="42"/>
-      <c r="AA52" s="43"/>
-      <c r="AB52" s="42"/>
-      <c r="AM52" s="43"/>
-      <c r="AN52" s="42"/>
-      <c r="AY52" s="43"/>
+      <c r="D52" s="26"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="26"/>
+      <c r="AA52" s="27"/>
+      <c r="AB52" s="26"/>
+      <c r="AM52" s="27"/>
+      <c r="AN52" s="26"/>
+      <c r="AY52" s="27"/>
     </row>
     <row r="53" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D53" s="42"/>
-      <c r="O53" s="43"/>
-      <c r="P53" s="42"/>
-      <c r="AA53" s="43"/>
-      <c r="AB53" s="42"/>
-      <c r="AM53" s="43"/>
-      <c r="AN53" s="42"/>
-      <c r="AY53" s="43"/>
+      <c r="D53" s="26"/>
+      <c r="O53" s="27"/>
+      <c r="P53" s="26"/>
+      <c r="AA53" s="27"/>
+      <c r="AB53" s="26"/>
+      <c r="AM53" s="27"/>
+      <c r="AN53" s="26"/>
+      <c r="AY53" s="27"/>
     </row>
     <row r="54" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D54" s="42"/>
-      <c r="O54" s="43"/>
-      <c r="P54" s="42"/>
-      <c r="AA54" s="43"/>
-      <c r="AB54" s="42"/>
-      <c r="AM54" s="43"/>
-      <c r="AN54" s="42"/>
-      <c r="AY54" s="43"/>
+      <c r="D54" s="26"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="26"/>
+      <c r="AA54" s="27"/>
+      <c r="AB54" s="26"/>
+      <c r="AM54" s="27"/>
+      <c r="AN54" s="26"/>
+      <c r="AY54" s="27"/>
     </row>
     <row r="55" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D55" s="42"/>
-      <c r="O55" s="43"/>
-      <c r="P55" s="42"/>
-      <c r="AA55" s="43"/>
-      <c r="AB55" s="42"/>
-      <c r="AM55" s="43"/>
-      <c r="AN55" s="42"/>
-      <c r="AY55" s="43"/>
+      <c r="D55" s="26"/>
+      <c r="O55" s="27"/>
+      <c r="P55" s="26"/>
+      <c r="AA55" s="27"/>
+      <c r="AB55" s="26"/>
+      <c r="AM55" s="27"/>
+      <c r="AN55" s="26"/>
+      <c r="AY55" s="27"/>
     </row>
     <row r="56" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D56" s="42"/>
-      <c r="O56" s="43"/>
-      <c r="P56" s="42"/>
-      <c r="AA56" s="43"/>
-      <c r="AB56" s="42"/>
-      <c r="AM56" s="43"/>
-      <c r="AN56" s="42"/>
-      <c r="AY56" s="43"/>
+      <c r="D56" s="26"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="26"/>
+      <c r="AA56" s="27"/>
+      <c r="AB56" s="26"/>
+      <c r="AM56" s="27"/>
+      <c r="AN56" s="26"/>
+      <c r="AY56" s="27"/>
     </row>
     <row r="57" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D57" s="42"/>
-      <c r="O57" s="43"/>
-      <c r="P57" s="42"/>
-      <c r="AA57" s="43"/>
-      <c r="AB57" s="42"/>
-      <c r="AM57" s="43"/>
-      <c r="AN57" s="42"/>
-      <c r="AY57" s="43"/>
+      <c r="D57" s="26"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="26"/>
+      <c r="AA57" s="27"/>
+      <c r="AB57" s="26"/>
+      <c r="AM57" s="27"/>
+      <c r="AN57" s="26"/>
+      <c r="AY57" s="27"/>
     </row>
     <row r="58" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D58" s="42"/>
-      <c r="O58" s="43"/>
-      <c r="P58" s="42"/>
-      <c r="AA58" s="43"/>
-      <c r="AB58" s="42"/>
-      <c r="AM58" s="43"/>
-      <c r="AN58" s="42"/>
-      <c r="AY58" s="43"/>
+      <c r="D58" s="26"/>
+      <c r="O58" s="27"/>
+      <c r="P58" s="26"/>
+      <c r="AA58" s="27"/>
+      <c r="AB58" s="26"/>
+      <c r="AM58" s="27"/>
+      <c r="AN58" s="26"/>
+      <c r="AY58" s="27"/>
     </row>
     <row r="59" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D59" s="42"/>
-      <c r="O59" s="43"/>
-      <c r="P59" s="42"/>
-      <c r="AA59" s="43"/>
-      <c r="AB59" s="42"/>
-      <c r="AM59" s="43"/>
-      <c r="AN59" s="42"/>
-      <c r="AY59" s="43"/>
+      <c r="D59" s="26"/>
+      <c r="O59" s="27"/>
+      <c r="P59" s="26"/>
+      <c r="AA59" s="27"/>
+      <c r="AB59" s="26"/>
+      <c r="AM59" s="27"/>
+      <c r="AN59" s="26"/>
+      <c r="AY59" s="27"/>
     </row>
     <row r="60" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D60" s="42"/>
-      <c r="O60" s="43"/>
-      <c r="P60" s="42"/>
-      <c r="AA60" s="43"/>
-      <c r="AB60" s="42"/>
-      <c r="AM60" s="43"/>
-      <c r="AN60" s="42"/>
-      <c r="AY60" s="43"/>
+      <c r="D60" s="26"/>
+      <c r="O60" s="27"/>
+      <c r="P60" s="26"/>
+      <c r="AA60" s="27"/>
+      <c r="AB60" s="26"/>
+      <c r="AM60" s="27"/>
+      <c r="AN60" s="26"/>
+      <c r="AY60" s="27"/>
     </row>
     <row r="61" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D61" s="42"/>
-      <c r="O61" s="43"/>
-      <c r="P61" s="42"/>
-      <c r="AA61" s="43"/>
-      <c r="AB61" s="42"/>
-      <c r="AM61" s="43"/>
-      <c r="AN61" s="42"/>
-      <c r="AY61" s="43"/>
+      <c r="D61" s="26"/>
+      <c r="O61" s="27"/>
+      <c r="P61" s="26"/>
+      <c r="AA61" s="27"/>
+      <c r="AB61" s="26"/>
+      <c r="AM61" s="27"/>
+      <c r="AN61" s="26"/>
+      <c r="AY61" s="27"/>
     </row>
     <row r="62" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D62" s="42"/>
-      <c r="O62" s="43"/>
-      <c r="P62" s="42"/>
-      <c r="AA62" s="43"/>
-      <c r="AB62" s="42"/>
-      <c r="AM62" s="43"/>
-      <c r="AN62" s="42"/>
-      <c r="AY62" s="43"/>
+      <c r="D62" s="26"/>
+      <c r="O62" s="27"/>
+      <c r="P62" s="26"/>
+      <c r="AA62" s="27"/>
+      <c r="AB62" s="26"/>
+      <c r="AM62" s="27"/>
+      <c r="AN62" s="26"/>
+      <c r="AY62" s="27"/>
     </row>
     <row r="63" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D63" s="42"/>
-      <c r="O63" s="43"/>
-      <c r="P63" s="42"/>
-      <c r="AA63" s="43"/>
-      <c r="AB63" s="42"/>
-      <c r="AM63" s="43"/>
-      <c r="AN63" s="42"/>
-      <c r="AY63" s="43"/>
+      <c r="D63" s="26"/>
+      <c r="O63" s="27"/>
+      <c r="P63" s="26"/>
+      <c r="AA63" s="27"/>
+      <c r="AB63" s="26"/>
+      <c r="AM63" s="27"/>
+      <c r="AN63" s="26"/>
+      <c r="AY63" s="27"/>
     </row>
     <row r="64" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D64" s="42"/>
-      <c r="O64" s="43"/>
-      <c r="P64" s="42"/>
-      <c r="AA64" s="43"/>
-      <c r="AB64" s="42"/>
-      <c r="AM64" s="43"/>
-      <c r="AN64" s="42"/>
-      <c r="AY64" s="43"/>
+      <c r="D64" s="26"/>
+      <c r="O64" s="27"/>
+      <c r="P64" s="26"/>
+      <c r="AA64" s="27"/>
+      <c r="AB64" s="26"/>
+      <c r="AM64" s="27"/>
+      <c r="AN64" s="26"/>
+      <c r="AY64" s="27"/>
     </row>
     <row r="65" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D65" s="42"/>
-      <c r="O65" s="43"/>
-      <c r="P65" s="42"/>
-      <c r="AA65" s="43"/>
-      <c r="AB65" s="42"/>
-      <c r="AM65" s="43"/>
-      <c r="AN65" s="42"/>
-      <c r="AY65" s="43"/>
+      <c r="D65" s="26"/>
+      <c r="O65" s="27"/>
+      <c r="P65" s="26"/>
+      <c r="AA65" s="27"/>
+      <c r="AB65" s="26"/>
+      <c r="AM65" s="27"/>
+      <c r="AN65" s="26"/>
+      <c r="AY65" s="27"/>
     </row>
     <row r="66" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D66" s="42"/>
-      <c r="O66" s="43"/>
-      <c r="P66" s="42"/>
-      <c r="AA66" s="43"/>
-      <c r="AB66" s="42"/>
-      <c r="AM66" s="43"/>
-      <c r="AN66" s="42"/>
-      <c r="AY66" s="43"/>
+      <c r="D66" s="26"/>
+      <c r="O66" s="27"/>
+      <c r="P66" s="26"/>
+      <c r="AA66" s="27"/>
+      <c r="AB66" s="26"/>
+      <c r="AM66" s="27"/>
+      <c r="AN66" s="26"/>
+      <c r="AY66" s="27"/>
     </row>
     <row r="67" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D67" s="42"/>
-      <c r="O67" s="43"/>
-      <c r="P67" s="42"/>
-      <c r="AA67" s="43"/>
-      <c r="AB67" s="42"/>
-      <c r="AM67" s="43"/>
-      <c r="AN67" s="42"/>
-      <c r="AY67" s="43"/>
+      <c r="D67" s="26"/>
+      <c r="O67" s="27"/>
+      <c r="P67" s="26"/>
+      <c r="AA67" s="27"/>
+      <c r="AB67" s="26"/>
+      <c r="AM67" s="27"/>
+      <c r="AN67" s="26"/>
+      <c r="AY67" s="27"/>
     </row>
     <row r="68" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D68" s="42"/>
-      <c r="O68" s="43"/>
-      <c r="P68" s="42"/>
-      <c r="AA68" s="43"/>
-      <c r="AB68" s="42"/>
-      <c r="AM68" s="43"/>
-      <c r="AN68" s="42"/>
-      <c r="AY68" s="43"/>
+      <c r="D68" s="26"/>
+      <c r="O68" s="27"/>
+      <c r="P68" s="26"/>
+      <c r="AA68" s="27"/>
+      <c r="AB68" s="26"/>
+      <c r="AM68" s="27"/>
+      <c r="AN68" s="26"/>
+      <c r="AY68" s="27"/>
     </row>
     <row r="69" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D69" s="42"/>
-      <c r="O69" s="43"/>
-      <c r="P69" s="42"/>
-      <c r="AA69" s="43"/>
-      <c r="AB69" s="42"/>
-      <c r="AM69" s="43"/>
-      <c r="AN69" s="42"/>
-      <c r="AY69" s="43"/>
+      <c r="D69" s="26"/>
+      <c r="O69" s="27"/>
+      <c r="P69" s="26"/>
+      <c r="AA69" s="27"/>
+      <c r="AB69" s="26"/>
+      <c r="AM69" s="27"/>
+      <c r="AN69" s="26"/>
+      <c r="AY69" s="27"/>
     </row>
     <row r="70" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D70" s="42"/>
-      <c r="O70" s="43"/>
-      <c r="P70" s="42"/>
-      <c r="AA70" s="43"/>
-      <c r="AB70" s="42"/>
-      <c r="AM70" s="43"/>
-      <c r="AN70" s="42"/>
-      <c r="AY70" s="43"/>
+      <c r="D70" s="26"/>
+      <c r="O70" s="27"/>
+      <c r="P70" s="26"/>
+      <c r="AA70" s="27"/>
+      <c r="AB70" s="26"/>
+      <c r="AM70" s="27"/>
+      <c r="AN70" s="26"/>
+      <c r="AY70" s="27"/>
     </row>
     <row r="71" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D71" s="42"/>
-      <c r="O71" s="43"/>
-      <c r="P71" s="42"/>
-      <c r="AA71" s="43"/>
-      <c r="AB71" s="42"/>
-      <c r="AM71" s="43"/>
-      <c r="AN71" s="42"/>
-      <c r="AY71" s="43"/>
+      <c r="D71" s="26"/>
+      <c r="O71" s="27"/>
+      <c r="P71" s="26"/>
+      <c r="AA71" s="27"/>
+      <c r="AB71" s="26"/>
+      <c r="AM71" s="27"/>
+      <c r="AN71" s="26"/>
+      <c r="AY71" s="27"/>
     </row>
     <row r="72" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D72" s="42"/>
-      <c r="O72" s="43"/>
-      <c r="P72" s="42"/>
-      <c r="AA72" s="43"/>
-      <c r="AB72" s="42"/>
-      <c r="AM72" s="43"/>
-      <c r="AN72" s="42"/>
-      <c r="AY72" s="43"/>
+      <c r="D72" s="26"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="26"/>
+      <c r="AA72" s="27"/>
+      <c r="AB72" s="26"/>
+      <c r="AM72" s="27"/>
+      <c r="AN72" s="26"/>
+      <c r="AY72" s="27"/>
     </row>
     <row r="73" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D73" s="42"/>
-      <c r="O73" s="43"/>
-      <c r="P73" s="42"/>
-      <c r="AA73" s="43"/>
-      <c r="AB73" s="42"/>
-      <c r="AM73" s="43"/>
-      <c r="AN73" s="42"/>
-      <c r="AY73" s="43"/>
+      <c r="D73" s="26"/>
+      <c r="O73" s="27"/>
+      <c r="P73" s="26"/>
+      <c r="AA73" s="27"/>
+      <c r="AB73" s="26"/>
+      <c r="AM73" s="27"/>
+      <c r="AN73" s="26"/>
+      <c r="AY73" s="27"/>
     </row>
     <row r="74" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D74" s="42"/>
-      <c r="O74" s="43"/>
-      <c r="P74" s="42"/>
-      <c r="AA74" s="43"/>
-      <c r="AB74" s="42"/>
-      <c r="AM74" s="43"/>
-      <c r="AN74" s="42"/>
-      <c r="AY74" s="43"/>
+      <c r="D74" s="26"/>
+      <c r="O74" s="27"/>
+      <c r="P74" s="26"/>
+      <c r="AA74" s="27"/>
+      <c r="AB74" s="26"/>
+      <c r="AM74" s="27"/>
+      <c r="AN74" s="26"/>
+      <c r="AY74" s="27"/>
     </row>
     <row r="75" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D75" s="42"/>
-      <c r="O75" s="43"/>
-      <c r="P75" s="42"/>
-      <c r="AA75" s="43"/>
-      <c r="AB75" s="42"/>
-      <c r="AM75" s="43"/>
-      <c r="AN75" s="42"/>
-      <c r="AY75" s="43"/>
+      <c r="D75" s="26"/>
+      <c r="O75" s="27"/>
+      <c r="P75" s="26"/>
+      <c r="AA75" s="27"/>
+      <c r="AB75" s="26"/>
+      <c r="AM75" s="27"/>
+      <c r="AN75" s="26"/>
+      <c r="AY75" s="27"/>
     </row>
     <row r="76" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D76" s="42"/>
-      <c r="O76" s="43"/>
-      <c r="P76" s="42"/>
-      <c r="AA76" s="43"/>
-      <c r="AB76" s="42"/>
-      <c r="AM76" s="43"/>
-      <c r="AN76" s="42"/>
-      <c r="AY76" s="43"/>
+      <c r="D76" s="26"/>
+      <c r="O76" s="27"/>
+      <c r="P76" s="26"/>
+      <c r="AA76" s="27"/>
+      <c r="AB76" s="26"/>
+      <c r="AM76" s="27"/>
+      <c r="AN76" s="26"/>
+      <c r="AY76" s="27"/>
     </row>
     <row r="77" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D77" s="42"/>
-      <c r="O77" s="43"/>
-      <c r="P77" s="42"/>
-      <c r="AA77" s="43"/>
-      <c r="AB77" s="42"/>
-      <c r="AM77" s="43"/>
-      <c r="AN77" s="42"/>
-      <c r="AY77" s="43"/>
+      <c r="D77" s="26"/>
+      <c r="O77" s="27"/>
+      <c r="P77" s="26"/>
+      <c r="AA77" s="27"/>
+      <c r="AB77" s="26"/>
+      <c r="AM77" s="27"/>
+      <c r="AN77" s="26"/>
+      <c r="AY77" s="27"/>
     </row>
     <row r="78" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D78" s="42"/>
-      <c r="O78" s="43"/>
-      <c r="P78" s="42"/>
-      <c r="AA78" s="43"/>
-      <c r="AB78" s="42"/>
-      <c r="AM78" s="43"/>
-      <c r="AN78" s="42"/>
-      <c r="AY78" s="43"/>
+      <c r="D78" s="26"/>
+      <c r="O78" s="27"/>
+      <c r="P78" s="26"/>
+      <c r="AA78" s="27"/>
+      <c r="AB78" s="26"/>
+      <c r="AM78" s="27"/>
+      <c r="AN78" s="26"/>
+      <c r="AY78" s="27"/>
     </row>
     <row r="79" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D79" s="42"/>
-      <c r="O79" s="43"/>
-      <c r="P79" s="42"/>
-      <c r="AA79" s="43"/>
-      <c r="AB79" s="42"/>
-      <c r="AM79" s="43"/>
-      <c r="AN79" s="42"/>
-      <c r="AY79" s="43"/>
+      <c r="D79" s="26"/>
+      <c r="O79" s="27"/>
+      <c r="P79" s="26"/>
+      <c r="AA79" s="27"/>
+      <c r="AB79" s="26"/>
+      <c r="AM79" s="27"/>
+      <c r="AN79" s="26"/>
+      <c r="AY79" s="27"/>
     </row>
     <row r="80" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D80" s="42"/>
-      <c r="O80" s="43"/>
-      <c r="P80" s="42"/>
-      <c r="AA80" s="43"/>
-      <c r="AB80" s="42"/>
-      <c r="AM80" s="43"/>
-      <c r="AN80" s="42"/>
-      <c r="AY80" s="43"/>
+      <c r="D80" s="26"/>
+      <c r="O80" s="27"/>
+      <c r="P80" s="26"/>
+      <c r="AA80" s="27"/>
+      <c r="AB80" s="26"/>
+      <c r="AM80" s="27"/>
+      <c r="AN80" s="26"/>
+      <c r="AY80" s="27"/>
     </row>
     <row r="81" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D81" s="42"/>
-      <c r="O81" s="43"/>
-      <c r="P81" s="42"/>
-      <c r="AA81" s="43"/>
-      <c r="AB81" s="42"/>
-      <c r="AM81" s="43"/>
-      <c r="AN81" s="42"/>
-      <c r="AY81" s="43"/>
+      <c r="D81" s="26"/>
+      <c r="O81" s="27"/>
+      <c r="P81" s="26"/>
+      <c r="AA81" s="27"/>
+      <c r="AB81" s="26"/>
+      <c r="AM81" s="27"/>
+      <c r="AN81" s="26"/>
+      <c r="AY81" s="27"/>
     </row>
     <row r="82" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D82" s="42"/>
-      <c r="O82" s="43"/>
-      <c r="P82" s="42"/>
-      <c r="AA82" s="43"/>
-      <c r="AB82" s="42"/>
-      <c r="AM82" s="43"/>
-      <c r="AN82" s="42"/>
-      <c r="AY82" s="43"/>
+      <c r="D82" s="26"/>
+      <c r="O82" s="27"/>
+      <c r="P82" s="26"/>
+      <c r="AA82" s="27"/>
+      <c r="AB82" s="26"/>
+      <c r="AM82" s="27"/>
+      <c r="AN82" s="26"/>
+      <c r="AY82" s="27"/>
     </row>
     <row r="83" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D83" s="42"/>
-      <c r="O83" s="43"/>
-      <c r="P83" s="42"/>
-      <c r="AA83" s="43"/>
-      <c r="AB83" s="42"/>
-      <c r="AM83" s="43"/>
-      <c r="AN83" s="42"/>
-      <c r="AY83" s="43"/>
+      <c r="D83" s="26"/>
+      <c r="O83" s="27"/>
+      <c r="P83" s="26"/>
+      <c r="AA83" s="27"/>
+      <c r="AB83" s="26"/>
+      <c r="AM83" s="27"/>
+      <c r="AN83" s="26"/>
+      <c r="AY83" s="27"/>
     </row>
     <row r="84" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D84" s="42"/>
-      <c r="O84" s="43"/>
-      <c r="P84" s="42"/>
-      <c r="AA84" s="43"/>
-      <c r="AB84" s="42"/>
-      <c r="AM84" s="43"/>
-      <c r="AN84" s="42"/>
-      <c r="AY84" s="43"/>
+      <c r="D84" s="26"/>
+      <c r="O84" s="27"/>
+      <c r="P84" s="26"/>
+      <c r="AA84" s="27"/>
+      <c r="AB84" s="26"/>
+      <c r="AM84" s="27"/>
+      <c r="AN84" s="26"/>
+      <c r="AY84" s="27"/>
     </row>
     <row r="85" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D85" s="42"/>
-      <c r="O85" s="43"/>
-      <c r="P85" s="42"/>
-      <c r="AA85" s="43"/>
-      <c r="AB85" s="42"/>
-      <c r="AM85" s="43"/>
-      <c r="AN85" s="42"/>
-      <c r="AY85" s="43"/>
+      <c r="D85" s="26"/>
+      <c r="O85" s="27"/>
+      <c r="P85" s="26"/>
+      <c r="AA85" s="27"/>
+      <c r="AB85" s="26"/>
+      <c r="AM85" s="27"/>
+      <c r="AN85" s="26"/>
+      <c r="AY85" s="27"/>
     </row>
     <row r="86" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D86" s="42"/>
-      <c r="O86" s="43"/>
-      <c r="P86" s="42"/>
-      <c r="AA86" s="43"/>
-      <c r="AB86" s="42"/>
-      <c r="AM86" s="43"/>
-      <c r="AN86" s="42"/>
-      <c r="AY86" s="43"/>
+      <c r="D86" s="26"/>
+      <c r="O86" s="27"/>
+      <c r="P86" s="26"/>
+      <c r="AA86" s="27"/>
+      <c r="AB86" s="26"/>
+      <c r="AM86" s="27"/>
+      <c r="AN86" s="26"/>
+      <c r="AY86" s="27"/>
     </row>
     <row r="87" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D87" s="42"/>
-      <c r="O87" s="43"/>
-      <c r="P87" s="42"/>
-      <c r="AA87" s="43"/>
-      <c r="AB87" s="42"/>
-      <c r="AM87" s="43"/>
-      <c r="AN87" s="42"/>
-      <c r="AY87" s="43"/>
+      <c r="D87" s="26"/>
+      <c r="O87" s="27"/>
+      <c r="P87" s="26"/>
+      <c r="AA87" s="27"/>
+      <c r="AB87" s="26"/>
+      <c r="AM87" s="27"/>
+      <c r="AN87" s="26"/>
+      <c r="AY87" s="27"/>
     </row>
     <row r="88" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D88" s="42"/>
-      <c r="O88" s="43"/>
-      <c r="P88" s="42"/>
-      <c r="AA88" s="43"/>
-      <c r="AB88" s="42"/>
-      <c r="AM88" s="43"/>
-      <c r="AN88" s="42"/>
-      <c r="AY88" s="43"/>
+      <c r="D88" s="26"/>
+      <c r="O88" s="27"/>
+      <c r="P88" s="26"/>
+      <c r="AA88" s="27"/>
+      <c r="AB88" s="26"/>
+      <c r="AM88" s="27"/>
+      <c r="AN88" s="26"/>
+      <c r="AY88" s="27"/>
     </row>
     <row r="89" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D89" s="42"/>
-      <c r="O89" s="43"/>
-      <c r="P89" s="42"/>
-      <c r="AA89" s="43"/>
-      <c r="AB89" s="42"/>
-      <c r="AM89" s="43"/>
-      <c r="AN89" s="42"/>
-      <c r="AY89" s="43"/>
+      <c r="D89" s="26"/>
+      <c r="O89" s="27"/>
+      <c r="P89" s="26"/>
+      <c r="AA89" s="27"/>
+      <c r="AB89" s="26"/>
+      <c r="AM89" s="27"/>
+      <c r="AN89" s="26"/>
+      <c r="AY89" s="27"/>
     </row>
     <row r="90" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D90" s="42"/>
-      <c r="O90" s="43"/>
-      <c r="P90" s="42"/>
-      <c r="AA90" s="43"/>
-      <c r="AB90" s="42"/>
-      <c r="AM90" s="43"/>
-      <c r="AN90" s="42"/>
-      <c r="AY90" s="43"/>
+      <c r="D90" s="26"/>
+      <c r="O90" s="27"/>
+      <c r="P90" s="26"/>
+      <c r="AA90" s="27"/>
+      <c r="AB90" s="26"/>
+      <c r="AM90" s="27"/>
+      <c r="AN90" s="26"/>
+      <c r="AY90" s="27"/>
     </row>
     <row r="91" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D91" s="42"/>
-      <c r="O91" s="43"/>
-      <c r="P91" s="42"/>
-      <c r="AA91" s="43"/>
-      <c r="AB91" s="42"/>
-      <c r="AM91" s="43"/>
-      <c r="AN91" s="42"/>
-      <c r="AY91" s="43"/>
+      <c r="D91" s="26"/>
+      <c r="O91" s="27"/>
+      <c r="P91" s="26"/>
+      <c r="AA91" s="27"/>
+      <c r="AB91" s="26"/>
+      <c r="AM91" s="27"/>
+      <c r="AN91" s="26"/>
+      <c r="AY91" s="27"/>
     </row>
     <row r="92" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D92" s="42"/>
-      <c r="O92" s="43"/>
-      <c r="P92" s="42"/>
-      <c r="AA92" s="43"/>
-      <c r="AB92" s="42"/>
-      <c r="AM92" s="43"/>
-      <c r="AN92" s="42"/>
-      <c r="AY92" s="43"/>
+      <c r="D92" s="26"/>
+      <c r="O92" s="27"/>
+      <c r="P92" s="26"/>
+      <c r="AA92" s="27"/>
+      <c r="AB92" s="26"/>
+      <c r="AM92" s="27"/>
+      <c r="AN92" s="26"/>
+      <c r="AY92" s="27"/>
     </row>
     <row r="93" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D93" s="42"/>
-      <c r="O93" s="43"/>
-      <c r="P93" s="42"/>
-      <c r="AA93" s="43"/>
-      <c r="AB93" s="42"/>
-      <c r="AM93" s="43"/>
-      <c r="AN93" s="42"/>
-      <c r="AY93" s="43"/>
+      <c r="D93" s="26"/>
+      <c r="O93" s="27"/>
+      <c r="P93" s="26"/>
+      <c r="AA93" s="27"/>
+      <c r="AB93" s="26"/>
+      <c r="AM93" s="27"/>
+      <c r="AN93" s="26"/>
+      <c r="AY93" s="27"/>
     </row>
     <row r="94" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D94" s="42"/>
-      <c r="O94" s="43"/>
-      <c r="P94" s="42"/>
-      <c r="AA94" s="43"/>
-      <c r="AB94" s="42"/>
-      <c r="AM94" s="43"/>
-      <c r="AN94" s="42"/>
-      <c r="AY94" s="43"/>
+      <c r="D94" s="26"/>
+      <c r="O94" s="27"/>
+      <c r="P94" s="26"/>
+      <c r="AA94" s="27"/>
+      <c r="AB94" s="26"/>
+      <c r="AM94" s="27"/>
+      <c r="AN94" s="26"/>
+      <c r="AY94" s="27"/>
     </row>
     <row r="95" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D95" s="42"/>
-      <c r="O95" s="43"/>
-      <c r="P95" s="42"/>
-      <c r="AA95" s="43"/>
-      <c r="AB95" s="42"/>
-      <c r="AM95" s="43"/>
-      <c r="AN95" s="42"/>
-      <c r="AY95" s="43"/>
+      <c r="D95" s="26"/>
+      <c r="O95" s="27"/>
+      <c r="P95" s="26"/>
+      <c r="AA95" s="27"/>
+      <c r="AB95" s="26"/>
+      <c r="AM95" s="27"/>
+      <c r="AN95" s="26"/>
+      <c r="AY95" s="27"/>
     </row>
     <row r="96" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D96" s="42"/>
-      <c r="O96" s="43"/>
-      <c r="P96" s="42"/>
-      <c r="AA96" s="43"/>
-      <c r="AB96" s="42"/>
-      <c r="AM96" s="43"/>
-      <c r="AN96" s="42"/>
-      <c r="AY96" s="43"/>
+      <c r="D96" s="26"/>
+      <c r="O96" s="27"/>
+      <c r="P96" s="26"/>
+      <c r="AA96" s="27"/>
+      <c r="AB96" s="26"/>
+      <c r="AM96" s="27"/>
+      <c r="AN96" s="26"/>
+      <c r="AY96" s="27"/>
     </row>
     <row r="97" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D97" s="42"/>
-      <c r="O97" s="43"/>
-      <c r="P97" s="42"/>
-      <c r="AA97" s="43"/>
-      <c r="AB97" s="42"/>
-      <c r="AM97" s="43"/>
-      <c r="AN97" s="42"/>
-      <c r="AY97" s="43"/>
+      <c r="D97" s="26"/>
+      <c r="O97" s="27"/>
+      <c r="P97" s="26"/>
+      <c r="AA97" s="27"/>
+      <c r="AB97" s="26"/>
+      <c r="AM97" s="27"/>
+      <c r="AN97" s="26"/>
+      <c r="AY97" s="27"/>
     </row>
     <row r="98" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D98" s="42"/>
-      <c r="O98" s="43"/>
-      <c r="P98" s="42"/>
-      <c r="AA98" s="43"/>
-      <c r="AB98" s="42"/>
-      <c r="AM98" s="43"/>
-      <c r="AN98" s="42"/>
-      <c r="AY98" s="43"/>
+      <c r="D98" s="26"/>
+      <c r="O98" s="27"/>
+      <c r="P98" s="26"/>
+      <c r="AA98" s="27"/>
+      <c r="AB98" s="26"/>
+      <c r="AM98" s="27"/>
+      <c r="AN98" s="26"/>
+      <c r="AY98" s="27"/>
     </row>
     <row r="99" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D99" s="42"/>
-      <c r="O99" s="43"/>
-      <c r="P99" s="42"/>
-      <c r="AA99" s="43"/>
-      <c r="AB99" s="42"/>
-      <c r="AM99" s="43"/>
-      <c r="AN99" s="42"/>
-      <c r="AY99" s="43"/>
+      <c r="D99" s="26"/>
+      <c r="O99" s="27"/>
+      <c r="P99" s="26"/>
+      <c r="AA99" s="27"/>
+      <c r="AB99" s="26"/>
+      <c r="AM99" s="27"/>
+      <c r="AN99" s="26"/>
+      <c r="AY99" s="27"/>
     </row>
     <row r="100" spans="4:51" x14ac:dyDescent="0.3">
-      <c r="D100" s="42"/>
-      <c r="O100" s="43"/>
-      <c r="P100" s="42"/>
-      <c r="AA100" s="43"/>
-      <c r="AB100" s="42"/>
-      <c r="AM100" s="43"/>
-      <c r="AN100" s="42"/>
-      <c r="AY100" s="43"/>
+      <c r="D100" s="26"/>
+      <c r="O100" s="27"/>
+      <c r="P100" s="26"/>
+      <c r="AA100" s="27"/>
+      <c r="AB100" s="26"/>
+      <c r="AM100" s="27"/>
+      <c r="AN100" s="26"/>
+      <c r="AY100" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4624,15 +4525,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4674,10 +4575,10 @@
         <v>229</v>
       </c>
       <c r="F3">
-        <v>1.7</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4697,7 +4598,7 @@
         <v>231</v>
       </c>
       <c r="F4">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -4720,7 +4621,7 @@
         <v>233</v>
       </c>
       <c r="F5">
-        <v>5.0999999999999996</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -4743,10 +4644,10 @@
         <v>235</v>
       </c>
       <c r="F6">
-        <v>4.5999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -4766,10 +4667,10 @@
         <v>237</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>